<commit_message>
Updated directory for testing
</commit_message>
<xml_diff>
--- a/data/input/tree/meaningfulness/ecology/weights_1_ecol.xlsx
+++ b/data/input/tree/meaningfulness/ecology/weights_1_ecol.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikonagengast/Desktop/Paper_MA/Paper_Recycling_3/AHP_Monte_Carlo/data/test_inputs/weights/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikonagengast/Desktop/Paper_MA/Paper_Recycling_3/AHP_Monte_Carlo/data/input/tree/meaningfulness/ecology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0742CCA5-BDCE-8440-93A0-B52DAACDD3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93438BD4-D11D-3446-AF2B-D3857211623B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19360" windowHeight="18440" xr2:uid="{B7E2081D-577B-684F-9742-E21C9EA83400}"/>
   </bookViews>
@@ -388,7 +388,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>